<commit_message>
opdateret med nyt materiale L3
</commit_message>
<xml_diff>
--- a/01-Introduction/simple_histogram_simulation.xlsx
+++ b/01-Introduction/simple_histogram_simulation.xlsx
@@ -1,41 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fcv495\OneDrive - University of Copenhagen\HetAgent2024\repo_offline\AdvMacroHet-main-2024\01-Introduction\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/zbp778_ku_dk/Documents/11. semester/Heterogenous agent models/AdvMacroHet-fork/01-Introduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="104" documentId="11_A2B3067062B01B12D466B8CC9183524623590E8A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB09524A-665B-465C-8FE4-9B02B74AAADD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
   <si>
     <t>a = 0</t>
   </si>
   <si>
     <t>a = 1</t>
-  </si>
-  <si>
-    <t>z = low</t>
-  </si>
-  <si>
-    <t>z = high</t>
   </si>
   <si>
     <t>\underline{D}</t>
@@ -46,11 +52,29 @@
   <si>
     <t xml:space="preserve">t = </t>
   </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>z_t-1 = low</t>
+  </si>
+  <si>
+    <t>z_t-1 = high</t>
+  </si>
+  <si>
+    <t>z_t= low</t>
+  </si>
+  <si>
+    <t>z_t= high</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -98,7 +122,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -113,10 +137,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,32 +423,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
-    <col min="5" max="5" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="6" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7"/>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="6"/>
-      <c r="F1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>0</v>
@@ -436,12 +464,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
@@ -449,7 +477,9 @@
       <c r="D3" s="4">
         <v>0</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F3" s="2">
         <f>C3*0.5+C4*0.5</f>
         <v>0.5</v>
@@ -459,9 +489,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -469,7 +499,9 @@
       <c r="D4" s="4">
         <v>0</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F4" s="2">
         <f>C4*0.5+C3*0.5</f>
         <v>0.5</v>
@@ -479,21 +511,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f>A3+1</f>
         <v>1</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
         <f>F3+G3</f>
@@ -502,7 +540,9 @@
       <c r="D6" s="2">
         <v>0</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F6" s="2">
         <f>C6*0.5+C7*0.5</f>
         <v>0.375</v>
@@ -511,10 +551,19 @@
         <f>D6*0.5+D7*0.5</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I6" t="s">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>0.5</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <f>F4*0.5</f>
@@ -524,7 +573,9 @@
         <f>F4*0.5+G4</f>
         <v>0.25</v>
       </c>
-      <c r="E7" s="3"/>
+      <c r="E7" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F7" s="2">
         <f>C7*0.5+C6*0.5</f>
         <v>0.375</v>
@@ -533,8 +584,11 @@
         <f>D7*0.5+D6*0.5</f>
         <v>0.125</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -542,13 +596,13 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <f>A6+1</f>
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C9" s="2">
         <f>F6+G6</f>
@@ -557,7 +611,9 @@
       <c r="D9" s="2">
         <v>0</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F9" s="2">
         <f>C9*0.5+C10*0.5</f>
         <v>0.34375</v>
@@ -567,11 +623,11 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2">
+        <v>8</v>
+      </c>
+      <c r="C10" s="8">
         <f>F7*0.5</f>
         <v>0.1875</v>
       </c>
@@ -579,7 +635,9 @@
         <f>F7*0.5+G7</f>
         <v>0.3125</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F10" s="2">
         <f>C10*0.5+C9*0.5</f>
         <v>0.34375</v>
@@ -589,7 +647,7 @@
         <v>0.15625</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -597,13 +655,13 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>A9+1</f>
         <v>3</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <f>F9+G9</f>
@@ -612,7 +670,9 @@
       <c r="D12" s="2">
         <v>0</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F12" s="2">
         <f>C12*0.5+C13*0.5</f>
         <v>0.3359375</v>
@@ -622,9 +682,9 @@
         <v>0.1640625</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <f>F10*0.5</f>
@@ -634,7 +694,9 @@
         <f>F10*0.5+G10</f>
         <v>0.328125</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F13" s="2">
         <f>C13*0.5+C12*0.5</f>
         <v>0.3359375</v>
@@ -644,7 +706,7 @@
         <v>0.1640625</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="5"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -652,13 +714,13 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <f>A12+1</f>
         <v>4</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <f>F12+G12</f>
@@ -667,7 +729,9 @@
       <c r="D15" s="2">
         <v>0</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F15" s="2">
         <f>C15*0.5+C16*0.5</f>
         <v>0.333984375</v>
@@ -677,9 +741,9 @@
         <v>0.166015625</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C16" s="2">
         <f>F13*0.5</f>
@@ -689,7 +753,9 @@
         <f>F13*0.5+G13</f>
         <v>0.33203125</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F16" s="2">
         <f>C16*0.5+C15*0.5</f>
         <v>0.333984375</v>
@@ -713,7 +779,7 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2">
         <f>F15+G15</f>
@@ -722,7 +788,9 @@
       <c r="D18" s="2">
         <v>0</v>
       </c>
-      <c r="E18" s="3"/>
+      <c r="E18" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F18" s="2">
         <f>C18*0.5+C19*0.5</f>
         <v>0.33349609375</v>
@@ -734,7 +802,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C19" s="2">
         <f>F16*0.5</f>
@@ -744,7 +812,9 @@
         <f>F16*0.5+G16</f>
         <v>0.3330078125</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F19" s="2">
         <f>C19*0.5+C18*0.5</f>
         <v>0.33349609375</v>
@@ -768,7 +838,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
         <f>F18+G18</f>
@@ -777,7 +847,9 @@
       <c r="D21" s="2">
         <v>0</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F21" s="2">
         <f>C21*0.5+C22*0.5</f>
         <v>0.3333740234375</v>
@@ -789,7 +861,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C22" s="2">
         <f>F19*0.5</f>
@@ -799,7 +871,9 @@
         <f>F19*0.5+G19</f>
         <v>0.333251953125</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F22" s="2">
         <f>C22*0.5+C21*0.5</f>
         <v>0.3333740234375</v>
@@ -823,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C24" s="2">
         <f>F21+G21</f>
@@ -832,7 +906,9 @@
       <c r="D24" s="2">
         <v>0</v>
       </c>
-      <c r="E24" s="3"/>
+      <c r="E24" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F24" s="2">
         <f>C24*0.5+C25*0.5</f>
         <v>0.333343505859375</v>
@@ -844,7 +920,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C25" s="2">
         <f>F22*0.5</f>
@@ -854,7 +930,9 @@
         <f>F22*0.5+G22</f>
         <v>0.33331298828125</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F25" s="2">
         <f>C25*0.5+C24*0.5</f>
         <v>0.333343505859375</v>
@@ -878,7 +956,7 @@
         <v>8</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C27" s="2">
         <f>F24+G24</f>
@@ -887,7 +965,9 @@
       <c r="D27" s="2">
         <v>0</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F27" s="2">
         <f>C27*0.5+C28*0.5</f>
         <v>0.33333587646484375</v>
@@ -899,7 +979,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C28" s="2">
         <f>F25*0.5</f>
@@ -909,7 +989,9 @@
         <f>F25*0.5+G25</f>
         <v>0.3333282470703125</v>
       </c>
-      <c r="E28" s="3"/>
+      <c r="E28" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F28" s="2">
         <f>C28*0.5+C27*0.5</f>
         <v>0.33333587646484375</v>
@@ -933,7 +1015,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C30" s="2">
         <f>F27+G27</f>
@@ -942,7 +1024,9 @@
       <c r="D30" s="2">
         <v>0</v>
       </c>
-      <c r="E30" s="3"/>
+      <c r="E30" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F30" s="2">
         <f>C30*0.5+C31*0.5</f>
         <v>0.33333396911621094</v>
@@ -954,7 +1038,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C31" s="2">
         <f>F28*0.5</f>
@@ -964,7 +1048,9 @@
         <f>F28*0.5+G28</f>
         <v>0.33333206176757813</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F31" s="2">
         <f>C31*0.5+C30*0.5</f>
         <v>0.33333396911621094</v>
@@ -988,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C33" s="2">
         <f>F30+G30</f>
@@ -997,7 +1083,9 @@
       <c r="D33" s="2">
         <v>0</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="F33" s="2">
         <f>C33*0.5+C34*0.5</f>
         <v>0.33333349227905273</v>
@@ -1009,7 +1097,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B34" s="5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C34" s="2">
         <f>F31*0.5</f>
@@ -1019,7 +1107,9 @@
         <f>F31*0.5+G31</f>
         <v>0.33333301544189453</v>
       </c>
-      <c r="E34" s="3"/>
+      <c r="E34" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="F34" s="2">
         <f>C34*0.5+C33*0.5</f>
         <v>0.33333349227905273</v>
@@ -1051,7 +1141,7 @@
       <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C38" s="7"/>
+      <c r="C38" s="6"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>

</xml_diff>